<commit_message>
Change some things in the excel file
</commit_message>
<xml_diff>
--- a/output/results/datasets.xlsx
+++ b/output/results/datasets.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Yannick/Documents/RA work/output/results/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Yannick/Documents/LUC_github/VOC_land_use/output/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E770CC5F-98D9-B94C-8B46-92E21A9CE94D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41EFD244-4A31-8944-BA48-7B1AC5325B39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16080" xr2:uid="{506D5015-EA0E-A24A-8848-D6F7EA59D6E2}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6417" uniqueCount="778">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6437" uniqueCount="798">
   <si>
     <t>yes</t>
   </si>
@@ -2378,13 +2378,73 @@
   </si>
   <si>
     <t>roeroeloewe</t>
+  </si>
+  <si>
+    <t>Aggregation level</t>
+  </si>
+  <si>
+    <t>Research approach</t>
+  </si>
+  <si>
+    <t>Placename</t>
+  </si>
+  <si>
+    <t>The placenames can be portrayed on the map using the fuzzy approach, however it is not possible to assess the results. In this study LU tables that only specify a placename are not transcribed and therefore not used as they were not deemed useful for developing the methodology.</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>Can be used if the geographic location of the region is known. This can be found either through maps or through the clustering approach as long as there is at least a placename and region mentioned. In this study LU tables that only specify a Region are not transcribed and not used as they were not deemed useful for developing the methodology.</t>
+  </si>
+  <si>
+    <t>Subregion</t>
+  </si>
+  <si>
+    <t>Can be used if the geographic location of the subregion is known. This can be found either through maps or through the clustering approach as long as there is at least a placename and a subregion are mentioned. In this study LU tables that only specify a subregion are not transcribed and not used as they were not deemed useful for developing the methodology.</t>
+  </si>
+  <si>
+    <t>Placename + Subregion</t>
+  </si>
+  <si>
+    <t>Both approaches can be used. Firstly the clustering approach can be used to portray the subregion on the map. The fuzzy approach can also be used if the goal is to georeference the data to the village level. In this study LU tables that specify a placename and subregion are not transcribed since there were many duplicate names in the subregions and it was therefore impossible to portray the subregions on the map correctly and the tables were therefore not deemed useful for developing the methodology.</t>
+  </si>
+  <si>
+    <t>Region + Subregion</t>
+  </si>
+  <si>
+    <t>Can be used if the geographic location of the region and/or subregion is known. These can be found either through maps or through the clustering approach as long as there is at least a placename and a subregion are mentioned. In this study LU tables that only specify a subregion and a region are not transcribed and not used as they were not deemed useful for developing the methodology.</t>
+  </si>
+  <si>
+    <t>Placename + Region</t>
+  </si>
+  <si>
+    <t>Both approaches can be used. Firstly the clustering approach can be used to portray the region on the map. To directly use the jupyter notebooks, in the Excel file the Region should then be regarded as the subregion and the overarching region is for example the country. The fuzzy approach can also be used if the goal is to georeference the data to the village level. This last approach is taken in this study and the subregion is then transcribed as not_specified. It is not possible to assess the results of the fuzzy matching.</t>
+  </si>
+  <si>
+    <t>Placename + Region + Subregion</t>
+  </si>
+  <si>
+    <t>Both approaches can be used, and can be compared to assess the accuracy of the fuzzy matching procedure. This approach is taken in the study and a more elaborate explanation can be found in the texts. Applying both approaches allows for assessing the results of the fuzzy matching.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is the Excel template used in this study. The short_summary_of_datasets is both used to keep track of the assessed datasets in the text mining phase and is used to inform what sheets to include in the location matching phase. </t>
+  </si>
+  <si>
+    <t>On https://github.com/Yegberink/VOC_land_use the Jupyter notebooks connected to this excel can be found.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Your data might require some different measure to identify the already assessed documents. In that case change the label_number in the short_summary_of_datasets sheet and the label generation part of the keyword-based text mining jupyter notebook. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">In the table below you can find an overview of what approach to use and what to take into account when using your data. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2418,6 +2478,18 @@
       <color rgb="FF000000"/>
       <name val="Helvetica Neue"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -2583,7 +2655,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -2610,6 +2682,11 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3646,14 +3723,125 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32E705B2-B562-C24F-82B8-F0AFB1CB6766}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" zoomScale="107" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="125.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B1" s="26"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B2" s="26"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="26" t="s">
+        <v>794</v>
+      </c>
+      <c r="B3" s="26"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="26" t="s">
+        <v>795</v>
+      </c>
+      <c r="B4" s="26"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="26" t="s">
+        <v>796</v>
+      </c>
+      <c r="B5" s="26"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="26"/>
+      <c r="B6" s="26"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="26"/>
+      <c r="B7" s="26"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="26" t="s">
+        <v>797</v>
+      </c>
+      <c r="B8" s="26"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="26"/>
+      <c r="B9" s="26"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="27" t="s">
+        <v>778</v>
+      </c>
+      <c r="B10" s="27" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+      <c r="A11" s="27" t="s">
+        <v>780</v>
+      </c>
+      <c r="B11" s="28" t="s">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+      <c r="A12" s="27" t="s">
+        <v>782</v>
+      </c>
+      <c r="B12" s="28" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+      <c r="A13" s="27" t="s">
+        <v>784</v>
+      </c>
+      <c r="B13" s="28" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="85" x14ac:dyDescent="0.2">
+      <c r="A14" s="27" t="s">
+        <v>786</v>
+      </c>
+      <c r="B14" s="28" t="s">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+      <c r="A15" s="27" t="s">
+        <v>788</v>
+      </c>
+      <c r="B15" s="28" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="85" x14ac:dyDescent="0.2">
+      <c r="A16" s="27" t="s">
+        <v>790</v>
+      </c>
+      <c r="B16" s="28" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+      <c r="A17" s="27" t="s">
+        <v>792</v>
+      </c>
+      <c r="B17" s="28" t="s">
+        <v>793</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -23649,7 +23837,7 @@
         <v>187</v>
       </c>
       <c r="I162">
-        <f t="shared" ref="I162:I193" si="5">SUM(F162:H162)</f>
+        <f t="shared" ref="I162:I180" si="5">SUM(F162:H162)</f>
         <v>387</v>
       </c>
       <c r="J162" t="s">
@@ -28537,7 +28725,7 @@
         <v>144</v>
       </c>
       <c r="I130">
-        <f t="shared" ref="I130:I161" si="4">SUM(F130:H130)</f>
+        <f t="shared" ref="I130:I136" si="4">SUM(F130:H130)</f>
         <v>204</v>
       </c>
       <c r="J130" t="s">

</xml_diff>